<commit_message>
- accidentally deleted conda :( so here's a new venv - also added the first trained network :D
</commit_message>
<xml_diff>
--- a/Data/Excel/SAGA MERGE AERO.xlsx
+++ b/Data/Excel/SAGA MERGE AERO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SARP\SARP-Aerosol-ML-BrC\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EA890C-E8F2-4744-BAFC-E4A0C2FA23F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AB7B26-46F8-431B-975C-547125F08415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="11700" yWindow="2412" windowWidth="10284" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3882,13 +3882,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:TO606"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A474" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A574" workbookViewId="0">
+      <selection activeCell="A341" sqref="A341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="1" max="1" width="34" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:534" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
- added Jupyter Notebooks to isolate training and testing, and start rebuilding data processing pipeline
</commit_message>
<xml_diff>
--- a/Data/Excel/SAGA MERGE AERO.xlsx
+++ b/Data/Excel/SAGA MERGE AERO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SARP\SARP-Aerosol-ML-BrC\Data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AB7B26-46F8-431B-975C-547125F08415}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49573198-2E39-43E0-845F-4D2791EDF7A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="11700" yWindow="2412" windowWidth="10284" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3577,12 +3577,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -3597,9 +3603,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3882,8 +3889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:TO606"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A574" workbookViewId="0">
-      <selection activeCell="A341" sqref="A341"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A444" sqref="A444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7399,7 +7406,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B40" t="s">
@@ -7463,7 +7470,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="A48" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B48" t="s">
@@ -8135,7 +8142,7 @@
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
+      <c r="A132" s="2" t="s">
         <v>178</v>
       </c>
       <c r="B132" t="s">
@@ -8199,7 +8206,7 @@
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
+      <c r="A140" s="2" t="s">
         <v>186</v>
       </c>
       <c r="B140" t="s">
@@ -8207,7 +8214,7 @@
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
+      <c r="A141" s="2" t="s">
         <v>187</v>
       </c>
       <c r="B141" t="s">
@@ -8215,7 +8222,7 @@
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
+      <c r="A142" s="2" t="s">
         <v>188</v>
       </c>
       <c r="B142" t="s">
@@ -8223,7 +8230,7 @@
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
+      <c r="A143" s="2" t="s">
         <v>189</v>
       </c>
       <c r="B143" t="s">
@@ -8231,7 +8238,7 @@
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
+      <c r="A144" s="2" t="s">
         <v>190</v>
       </c>
       <c r="B144" t="s">
@@ -8239,7 +8246,7 @@
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
+      <c r="A145" s="2" t="s">
         <v>191</v>
       </c>
       <c r="B145" t="s">
@@ -8247,7 +8254,7 @@
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
+      <c r="A146" s="2" t="s">
         <v>192</v>
       </c>
       <c r="B146" t="s">
@@ -8255,7 +8262,7 @@
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
+      <c r="A147" s="2" t="s">
         <v>193</v>
       </c>
       <c r="B147" t="s">
@@ -9775,7 +9782,7 @@
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A337" t="s">
+      <c r="A337" s="2" t="s">
         <v>385</v>
       </c>
       <c r="B337" t="s">
@@ -9959,7 +9966,7 @@
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A360" t="s">
+      <c r="A360" s="2" t="s">
         <v>414</v>
       </c>
       <c r="B360" t="s">
@@ -9967,7 +9974,7 @@
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A361" t="s">
+      <c r="A361" s="2" t="s">
         <v>415</v>
       </c>
       <c r="B361" t="s">

</xml_diff>